<commit_message>
Ajout neutrinos + étoiles à neutrons + restauration climatique
</commit_message>
<xml_diff>
--- a/Arbretechno.xlsx
+++ b/Arbretechno.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dl028206\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Starempires\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EFC6F95F-967A-41FB-B103-675A3A4E74F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85EF53AE-344C-4682-9AA4-7CCD23CD9312}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2875B448-5379-4D18-8E88-FF8DB286F2B1}"/>
+    <workbookView minimized="1" xWindow="300" yWindow="15" windowWidth="16665" windowHeight="13695" xr2:uid="{2875B448-5379-4D18-8E88-FF8DB286F2B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Centre de recherche</t>
   </si>
@@ -127,6 +127,15 @@
   </si>
   <si>
     <t>Moteur III</t>
+  </si>
+  <si>
+    <t>Basemilitaire</t>
+  </si>
+  <si>
+    <t>Restauration planétaire</t>
+  </si>
+  <si>
+    <t>Amélioration planétaire</t>
   </si>
 </sst>
 </file>
@@ -225,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -252,6 +261,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -569,10 +584,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53110EFC-72E2-49A1-9CE8-0D104E704F77}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,15 +598,16 @@
     <col min="4" max="4" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.42578125" customWidth="1"/>
-    <col min="14" max="14" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.42578125" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -599,7 +615,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -607,48 +623,49 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11" t="s">
+      <c r="D4" s="12"/>
+      <c r="E4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="11"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F4" s="12"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -664,8 +681,9 @@
       <c r="F6" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G6" s="13"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -676,15 +694,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C8" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -697,19 +721,20 @@
       <c r="F9" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G9" s="13"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -718,12 +743,12 @@
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="8"/>
+      <c r="I11" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -733,73 +758,61 @@
       <c r="D12" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="H12" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="J13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="K13" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="I14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E4:F4"/>
-    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E7A3BE3C474AA34BAAFA089D2F0226F7" ma:contentTypeVersion="0" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="5592e3650de2659214febfddb0aef387">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5f46307b522de21dcbe8dbdcadb9a8cd">
     <xsd:element name="properties">
@@ -913,30 +926,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33E05040-E7C8-46DB-B74F-E82280DAD5A9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9EF8C0CB-595E-4A4E-9C5A-D6D4CB804B3E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{099BA056-84A5-466D-9745-99F645D9FE6E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -950,4 +955,27 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9EF8C0CB-595E-4A4E-9C5A-D6D4CB804B3E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33E05040-E7C8-46DB-B74F-E82280DAD5A9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>